<commit_message>
updated saft-gamma-mie database (extra amines-co2-h2o interactions)
</commit_message>
<xml_diff>
--- a/sgtpy/database/saftgamma_database.xlsx
+++ b/sgtpy/database/saftgamma_database.xlsx
@@ -18,7 +18,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="95">
+  <si>
+    <t>groups</t>
+  </si>
   <si>
     <t>vk*</t>
   </si>
@@ -57,9 +60,6 @@
   </si>
   <si>
     <t>mw_kk</t>
-  </si>
-  <si>
-    <t>groups</t>
   </si>
   <si>
     <t>CH3</t>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>R1CH3N[CH2 CH2OH]</t>
+  </si>
+  <si>
+    <t>[NHCH2CH2OH]2</t>
+  </si>
+  <si>
+    <t>[R(CH2)n]CH2OH; n = 0, 1, 2 (excluding butanol)</t>
+  </si>
+  <si>
+    <t>NH[CH2 CH2OH]2</t>
+  </si>
+  <si>
+    <t>R1CH3N[CH2 CH2OH]</t>
   </si>
 </sst>
 </file>
@@ -656,50 +668,50 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
@@ -743,7 +755,7 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
@@ -787,7 +799,7 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4">
@@ -831,7 +843,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5">
@@ -875,7 +887,7 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
@@ -919,7 +931,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
@@ -963,7 +975,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8">
@@ -1007,7 +1019,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
@@ -1051,7 +1063,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
@@ -1095,7 +1107,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11">
@@ -1139,7 +1151,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12">
@@ -1183,7 +1195,7 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13">
@@ -1227,7 +1239,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14">
@@ -1271,7 +1283,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15">
@@ -1315,7 +1327,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16">
@@ -1359,7 +1371,7 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17">
@@ -1403,7 +1415,7 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18">
@@ -1447,7 +1459,7 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19">
@@ -1491,7 +1503,7 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20">
@@ -1535,7 +1547,7 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21">
@@ -1579,7 +1591,7 @@
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
       <c r="B22">
@@ -1623,7 +1635,7 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23">
@@ -1667,7 +1679,7 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24">
@@ -1711,7 +1723,7 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25">
@@ -1755,7 +1767,7 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26">
@@ -1799,7 +1811,7 @@
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
       <c r="B27">
@@ -1843,7 +1855,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
       <c r="B28">
@@ -1887,7 +1899,7 @@
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
       <c r="B29">
@@ -1931,7 +1943,7 @@
       </c>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30">
@@ -1975,7 +1987,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
       <c r="B31">
@@ -2019,7 +2031,7 @@
       </c>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="B32">
@@ -2063,7 +2075,7 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33">
@@ -2107,7 +2119,7 @@
       </c>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
       <c r="B34">
@@ -2151,7 +2163,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35">
@@ -2195,7 +2207,7 @@
       </c>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
       <c r="B36">
@@ -2239,7 +2251,7 @@
       </c>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>49</v>
       </c>
       <c r="B37">
@@ -2283,7 +2295,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>50</v>
       </c>
       <c r="B38">
@@ -2327,7 +2339,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>51</v>
       </c>
       <c r="B39">
@@ -2371,7 +2383,7 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>52</v>
       </c>
       <c r="B40">
@@ -2415,7 +2427,7 @@
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>53</v>
       </c>
       <c r="B41">
@@ -2459,7 +2471,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>54</v>
       </c>
       <c r="B42">
@@ -2503,7 +2515,7 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>55</v>
       </c>
       <c r="B43">
@@ -2547,7 +2559,7 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>56</v>
       </c>
       <c r="B44">
@@ -2591,7 +2603,7 @@
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>57</v>
       </c>
       <c r="B45">
@@ -2635,7 +2647,7 @@
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>58</v>
       </c>
       <c r="B46">
@@ -2679,7 +2691,7 @@
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>59</v>
       </c>
       <c r="B47">
@@ -2723,7 +2735,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>60</v>
       </c>
       <c r="B48">
@@ -2767,7 +2779,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>61</v>
       </c>
       <c r="B49">
@@ -2811,7 +2823,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>62</v>
       </c>
       <c r="B50">
@@ -2855,7 +2867,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>63</v>
       </c>
       <c r="B51">
@@ -2899,7 +2911,7 @@
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>64</v>
       </c>
       <c r="B52">
@@ -2943,7 +2955,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>65</v>
       </c>
       <c r="B53">
@@ -2987,7 +2999,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>66</v>
       </c>
       <c r="B54">
@@ -3031,7 +3043,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>67</v>
       </c>
       <c r="B55">
@@ -3075,7 +3087,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>68</v>
       </c>
       <c r="B56">
@@ -3119,7 +3131,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
       <c r="B57">
@@ -3163,7 +3175,7 @@
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>70</v>
       </c>
       <c r="B58">
@@ -3207,7 +3219,7 @@
       </c>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>71</v>
       </c>
       <c r="B59">
@@ -3257,7 +3269,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D331"/>
+  <dimension ref="A1:D333"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7897,6 +7909,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="332" spans="1:4">
+      <c r="A332" t="s">
+        <v>44</v>
+      </c>
+      <c r="B332" t="s">
+        <v>30</v>
+      </c>
+      <c r="C332">
+        <v>161.38</v>
+      </c>
+      <c r="D332">
+        <v>33.269</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4">
+      <c r="A333" t="s">
+        <v>32</v>
+      </c>
+      <c r="B333" t="s">
+        <v>30</v>
+      </c>
+      <c r="C333">
+        <v>312.3</v>
+      </c>
+      <c r="D333" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7904,7 +7944,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10530,6 +10570,46 @@
         <v>47.677</v>
       </c>
     </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>44</v>
+      </c>
+      <c r="B132" t="s">
+        <v>81</v>
+      </c>
+      <c r="C132" t="s">
+        <v>30</v>
+      </c>
+      <c r="D132" t="s">
+        <v>81</v>
+      </c>
+      <c r="E132">
+        <v>4114.9</v>
+      </c>
+      <c r="F132">
+        <v>4686.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>44</v>
+      </c>
+      <c r="B133" t="s">
+        <v>81</v>
+      </c>
+      <c r="C133" t="s">
+        <v>30</v>
+      </c>
+      <c r="D133" t="s">
+        <v>83</v>
+      </c>
+      <c r="E133">
+        <v>1013.9</v>
+      </c>
+      <c r="F133">
+        <v>1551.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10537,7 +10617,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10696,6 +10776,23 @@
         <v>76</v>
       </c>
     </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10">
+        <v>488.28</v>
+      </c>
+      <c r="E10">
+        <v>49.901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10703,13 +10800,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -10723,13 +10820,16 @@
         <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -10742,14 +10842,17 @@
       <c r="D2" t="s">
         <v>81</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2">
         <v>600</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>490.19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -10762,14 +10865,17 @@
       <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3">
         <v>2000.6</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>130.02</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -10782,14 +10888,17 @@
       <c r="D4" t="s">
         <v>81</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4">
         <v>1364.4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>22.45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -10802,14 +10911,17 @@
       <c r="D5" t="s">
         <v>82</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5">
         <v>1877.5</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>459.18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -10822,14 +10934,17 @@
       <c r="D6" t="s">
         <v>81</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6">
         <v>3313</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3280.3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -10842,14 +10957,17 @@
       <c r="D7" t="s">
         <v>83</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7">
         <v>4943.6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>142.64</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -10862,14 +10980,17 @@
       <c r="D8" t="s">
         <v>81</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8">
         <v>629.88</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>346.08</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -10882,14 +11003,17 @@
       <c r="D9" t="s">
         <v>82</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9">
         <v>2403.8</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>26.192</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -10902,14 +11026,17 @@
       <c r="D10" t="s">
         <v>81</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10">
         <v>7020.9</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.0174</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -10922,14 +11049,17 @@
       <c r="D11" t="s">
         <v>83</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11">
         <v>2490.6</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>686.8200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -10942,14 +11072,17 @@
       <c r="D12" t="s">
         <v>82</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
         <v>1390.1</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>947.9299999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -10962,14 +11095,17 @@
       <c r="D13" t="s">
         <v>81</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13">
         <v>341.13</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1499.8</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -10982,14 +11118,17 @@
       <c r="D14" t="s">
         <v>82</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14">
         <v>2876.5</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.84013</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -11002,14 +11141,17 @@
       <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15">
         <v>5500.7</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1.3695</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -11022,14 +11164,17 @@
       <c r="D16" t="s">
         <v>83</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16">
         <v>3437.4</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2.767</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -11042,11 +11187,60 @@
       <c r="D17" t="s">
         <v>82</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17">
         <v>1210.9</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>950.4299999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18">
+        <v>305.8</v>
+      </c>
+      <c r="G18">
+        <v>0.011099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19">
+        <v>1756.2</v>
+      </c>
+      <c r="G19">
+        <v>24.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected NH-H2O association interaction
</commit_message>
<xml_diff>
--- a/sgtpy/database/saftgamma_database.xlsx
+++ b/sgtpy/database/saftgamma_database.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="116">
   <si>
     <t>groups</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>e2</t>
+  </si>
+  <si>
+    <t>felipe2021</t>
+  </si>
+  <si>
+    <t>10.1002/aic.17194</t>
   </si>
   <si>
     <t>environment</t>
@@ -12591,16 +12597,16 @@
         <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
         <v>100</v>
       </c>
       <c r="E50">
-        <v>3890.4</v>
+        <v>2783.7</v>
       </c>
       <c r="F50">
-        <v>928</v>
+        <v>15.536</v>
       </c>
       <c r="G50" t="s">
         <v>77</v>
@@ -12614,19 +12620,19 @@
         <v>29</v>
       </c>
       <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
         <v>101</v>
       </c>
-      <c r="C51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" t="s">
-        <v>100</v>
-      </c>
       <c r="E51">
-        <v>2783.7</v>
+        <v>1701</v>
       </c>
       <c r="F51">
-        <v>15.536</v>
+        <v>1.6177</v>
       </c>
       <c r="G51" t="s">
         <v>77</v>
@@ -12640,19 +12646,19 @@
         <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E52">
-        <v>1701</v>
+        <v>2838.4</v>
       </c>
       <c r="F52">
-        <v>1.6177</v>
+        <v>37.395</v>
       </c>
       <c r="G52" t="s">
         <v>77</v>
@@ -12669,16 +12675,16 @@
         <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
         <v>100</v>
       </c>
       <c r="E53">
-        <v>2838.4</v>
+        <v>5203.7</v>
       </c>
       <c r="F53">
-        <v>37.395</v>
+        <v>0.0374</v>
       </c>
       <c r="G53" t="s">
         <v>77</v>
@@ -12695,16 +12701,16 @@
         <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D54" t="s">
         <v>100</v>
       </c>
       <c r="E54">
-        <v>5203.7</v>
+        <v>563.5599999999999</v>
       </c>
       <c r="F54">
-        <v>0.0374</v>
+        <v>339.61</v>
       </c>
       <c r="G54" t="s">
         <v>77</v>
@@ -12718,19 +12724,19 @@
         <v>29</v>
       </c>
       <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" t="s">
         <v>101</v>
       </c>
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s">
-        <v>100</v>
-      </c>
       <c r="E55">
-        <v>563.5599999999999</v>
+        <v>2500</v>
       </c>
       <c r="F55">
-        <v>339.61</v>
+        <v>52.47</v>
       </c>
       <c r="G55" t="s">
         <v>77</v>
@@ -12744,19 +12750,19 @@
         <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
         <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56">
-        <v>2500</v>
+        <v>1798.2</v>
       </c>
       <c r="F56">
-        <v>52.47</v>
+        <v>103.92</v>
       </c>
       <c r="G56" t="s">
         <v>77</v>
@@ -12776,13 +12782,13 @@
         <v>43</v>
       </c>
       <c r="D57" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E57">
-        <v>1798.2</v>
+        <v>563.5599999999999</v>
       </c>
       <c r="F57">
-        <v>103.92</v>
+        <v>339.61</v>
       </c>
       <c r="G57" t="s">
         <v>77</v>
@@ -12799,16 +12805,16 @@
         <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E58">
-        <v>563.5599999999999</v>
+        <v>5903.8</v>
       </c>
       <c r="F58">
-        <v>339.61</v>
+        <v>0.002075</v>
       </c>
       <c r="G58" t="s">
         <v>77</v>
@@ -12822,19 +12828,19 @@
         <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
         <v>45</v>
       </c>
       <c r="D59" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E59">
-        <v>5903.8</v>
+        <v>5477.7</v>
       </c>
       <c r="F59">
-        <v>0.002075</v>
+        <v>0.009582</v>
       </c>
       <c r="G59" t="s">
         <v>77</v>
@@ -12848,19 +12854,19 @@
         <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E60">
-        <v>5477.7</v>
+        <v>4115.4</v>
       </c>
       <c r="F60">
-        <v>0.009582</v>
+        <v>0.2307</v>
       </c>
       <c r="G60" t="s">
         <v>77</v>
@@ -12874,19 +12880,19 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" t="s">
         <v>101</v>
       </c>
-      <c r="C61" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" t="s">
-        <v>100</v>
-      </c>
       <c r="E61">
-        <v>4115.4</v>
+        <v>1985.4</v>
       </c>
       <c r="F61">
-        <v>0.2307</v>
+        <v>101.69</v>
       </c>
       <c r="G61" t="s">
         <v>77</v>
@@ -12903,16 +12909,16 @@
         <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D62" t="s">
         <v>101</v>
       </c>
       <c r="E62">
-        <v>1985.4</v>
+        <v>2783.7</v>
       </c>
       <c r="F62">
-        <v>101.69</v>
+        <v>15.536</v>
       </c>
       <c r="G62" t="s">
         <v>77</v>
@@ -12926,19 +12932,19 @@
         <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E63">
-        <v>2783.7</v>
+        <v>1492</v>
       </c>
       <c r="F63">
-        <v>15.536</v>
+        <v>76.411</v>
       </c>
       <c r="G63" t="s">
         <v>77</v>
@@ -12955,16 +12961,16 @@
         <v>101</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D64" t="s">
         <v>100</v>
       </c>
       <c r="E64">
-        <v>1492</v>
+        <v>802.21</v>
       </c>
       <c r="F64">
-        <v>76.411</v>
+        <v>52.555</v>
       </c>
       <c r="G64" t="s">
         <v>77</v>
@@ -12981,16 +12987,16 @@
         <v>101</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
         <v>100</v>
       </c>
       <c r="E65">
-        <v>802.21</v>
+        <v>2900</v>
       </c>
       <c r="F65">
-        <v>52.555</v>
+        <v>38.401</v>
       </c>
       <c r="G65" t="s">
         <v>77</v>
@@ -13004,16 +13010,16 @@
         <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E66">
-        <v>2900</v>
+        <v>1606.6</v>
       </c>
       <c r="F66">
         <v>38.401</v>
@@ -13030,19 +13036,19 @@
         <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E67">
-        <v>1606.6</v>
+        <v>2350</v>
       </c>
       <c r="F67">
-        <v>38.401</v>
+        <v>97.014</v>
       </c>
       <c r="G67" t="s">
         <v>77</v>
@@ -13059,16 +13065,16 @@
         <v>101</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D68" t="s">
         <v>100</v>
       </c>
       <c r="E68">
-        <v>2350</v>
+        <v>1398.1</v>
       </c>
       <c r="F68">
-        <v>97.014</v>
+        <v>91.419</v>
       </c>
       <c r="G68" t="s">
         <v>77</v>
@@ -13085,16 +13091,16 @@
         <v>101</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D69" t="s">
         <v>100</v>
       </c>
       <c r="E69">
-        <v>1398.1</v>
+        <v>882.05</v>
       </c>
       <c r="F69">
-        <v>91.419</v>
+        <v>984.34</v>
       </c>
       <c r="G69" t="s">
         <v>77</v>
@@ -13114,7 +13120,7 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E70">
         <v>882.05</v>
@@ -13134,19 +13140,19 @@
         <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" t="s">
         <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E71">
-        <v>882.05</v>
+        <v>5192.5</v>
       </c>
       <c r="F71">
-        <v>984.34</v>
+        <v>0.011186</v>
       </c>
       <c r="G71" t="s">
         <v>77</v>
@@ -13157,22 +13163,22 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E72">
-        <v>5192.5</v>
+        <v>2062.1</v>
       </c>
       <c r="F72">
-        <v>0.011186</v>
+        <v>106.57</v>
       </c>
       <c r="G72" t="s">
         <v>77</v>
@@ -13189,16 +13195,16 @@
         <v>101</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="D73" t="s">
         <v>100</v>
       </c>
       <c r="E73">
-        <v>2062.1</v>
+        <v>1400.7</v>
       </c>
       <c r="F73">
-        <v>106.57</v>
+        <v>495.32</v>
       </c>
       <c r="G73" t="s">
         <v>77</v>
@@ -13212,19 +13218,19 @@
         <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
         <v>69</v>
       </c>
       <c r="D74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E74">
-        <v>1400.7</v>
+        <v>871.46</v>
       </c>
       <c r="F74">
-        <v>495.32</v>
+        <v>0.25605</v>
       </c>
       <c r="G74" t="s">
         <v>77</v>
@@ -13238,19 +13244,19 @@
         <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E75">
-        <v>871.46</v>
+        <v>2346</v>
       </c>
       <c r="F75">
-        <v>0.25605</v>
+        <v>3.1536</v>
       </c>
       <c r="G75" t="s">
         <v>77</v>
@@ -13264,13 +13270,13 @@
         <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
         <v>70</v>
       </c>
       <c r="D76" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E76">
         <v>2346</v>
@@ -13287,22 +13293,22 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B77" t="s">
         <v>100</v>
       </c>
       <c r="C77" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E77">
-        <v>2346</v>
+        <v>4023.9</v>
       </c>
       <c r="F77">
-        <v>3.1536</v>
+        <v>120.35</v>
       </c>
       <c r="G77" t="s">
         <v>77</v>
@@ -13316,7 +13322,7 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C78" t="s">
         <v>36</v>
@@ -13325,10 +13331,10 @@
         <v>100</v>
       </c>
       <c r="E78">
-        <v>4023.9</v>
+        <v>5981.4</v>
       </c>
       <c r="F78">
-        <v>120.35</v>
+        <v>1.0036</v>
       </c>
       <c r="G78" t="s">
         <v>77</v>
@@ -13342,19 +13348,19 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D79" t="s">
         <v>100</v>
       </c>
       <c r="E79">
-        <v>5981.4</v>
+        <v>6012.1</v>
       </c>
       <c r="F79">
-        <v>1.0036</v>
+        <v>0.14157</v>
       </c>
       <c r="G79" t="s">
         <v>77</v>
@@ -13368,7 +13374,7 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C80" t="s">
         <v>37</v>
@@ -13377,10 +13383,10 @@
         <v>100</v>
       </c>
       <c r="E80">
-        <v>6012.1</v>
+        <v>7420.5</v>
       </c>
       <c r="F80">
-        <v>0.14157</v>
+        <v>0.43534</v>
       </c>
       <c r="G80" t="s">
         <v>77</v>
@@ -13394,19 +13400,19 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D81" t="s">
         <v>100</v>
       </c>
       <c r="E81">
-        <v>7420.5</v>
+        <v>4270.8</v>
       </c>
       <c r="F81">
-        <v>0.43534</v>
+        <v>0.4634</v>
       </c>
       <c r="G81" t="s">
         <v>77</v>
@@ -13420,7 +13426,7 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C82" t="s">
         <v>38</v>
@@ -13429,10 +13435,10 @@
         <v>100</v>
       </c>
       <c r="E82">
-        <v>4270.8</v>
+        <v>7439.8</v>
       </c>
       <c r="F82">
-        <v>0.4634</v>
+        <v>0.006748</v>
       </c>
       <c r="G82" t="s">
         <v>77</v>
@@ -13446,19 +13452,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C83" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
         <v>100</v>
       </c>
       <c r="E83">
-        <v>7439.8</v>
+        <v>5696.6</v>
       </c>
       <c r="F83">
-        <v>0.006748</v>
+        <v>4.6758</v>
       </c>
       <c r="G83" t="s">
         <v>77</v>
@@ -13472,7 +13478,7 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C84" t="s">
         <v>39</v>
@@ -13481,10 +13487,10 @@
         <v>100</v>
       </c>
       <c r="E84">
-        <v>5696.6</v>
+        <v>6017.9</v>
       </c>
       <c r="F84">
-        <v>4.6758</v>
+        <v>1.1003</v>
       </c>
       <c r="G84" t="s">
         <v>77</v>
@@ -13498,19 +13504,19 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D85" t="s">
         <v>100</v>
       </c>
       <c r="E85">
-        <v>6017.9</v>
+        <v>3388.6</v>
       </c>
       <c r="F85">
-        <v>1.1003</v>
+        <v>1031</v>
       </c>
       <c r="G85" t="s">
         <v>77</v>
@@ -13524,7 +13530,7 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
         <v>40</v>
@@ -13533,10 +13539,10 @@
         <v>100</v>
       </c>
       <c r="E86">
-        <v>3388.6</v>
+        <v>3004.9</v>
       </c>
       <c r="F86">
-        <v>1031</v>
+        <v>659.21</v>
       </c>
       <c r="G86" t="s">
         <v>77</v>
@@ -13550,19 +13556,19 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D87" t="s">
         <v>100</v>
       </c>
       <c r="E87">
-        <v>3004.9</v>
+        <v>2246</v>
       </c>
       <c r="F87">
-        <v>659.21</v>
+        <v>0.14057</v>
       </c>
       <c r="G87" t="s">
         <v>77</v>
@@ -13576,7 +13582,7 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C88" t="s">
         <v>45</v>
@@ -13585,10 +13591,10 @@
         <v>100</v>
       </c>
       <c r="E88">
-        <v>2246</v>
+        <v>3870.8</v>
       </c>
       <c r="F88">
-        <v>0.14057</v>
+        <v>6445.7</v>
       </c>
       <c r="G88" t="s">
         <v>77</v>
@@ -13599,22 +13605,22 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
         <v>100</v>
       </c>
       <c r="E89">
-        <v>3870.8</v>
+        <v>2161</v>
       </c>
       <c r="F89">
-        <v>6445.7</v>
+        <v>54.398</v>
       </c>
       <c r="G89" t="s">
         <v>77</v>
@@ -13631,16 +13637,16 @@
         <v>101</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D90" t="s">
         <v>100</v>
       </c>
       <c r="E90">
-        <v>2161</v>
+        <v>1282.7</v>
       </c>
       <c r="F90">
-        <v>54.398</v>
+        <v>254.28</v>
       </c>
       <c r="G90" t="s">
         <v>77</v>
@@ -13654,19 +13660,19 @@
         <v>33</v>
       </c>
       <c r="B91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C91" t="s">
         <v>36</v>
       </c>
       <c r="D91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E91">
-        <v>1282.7</v>
+        <v>1354</v>
       </c>
       <c r="F91">
-        <v>254.28</v>
+        <v>141.35</v>
       </c>
       <c r="G91" t="s">
         <v>77</v>
@@ -13683,16 +13689,16 @@
         <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D92" t="s">
         <v>101</v>
       </c>
       <c r="E92">
-        <v>1354</v>
+        <v>861.12</v>
       </c>
       <c r="F92">
-        <v>141.35</v>
+        <v>556.3200000000001</v>
       </c>
       <c r="G92" t="s">
         <v>77</v>
@@ -13706,19 +13712,19 @@
         <v>33</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C93" t="s">
         <v>37</v>
       </c>
       <c r="D93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E93">
-        <v>861.12</v>
+        <v>1477.7</v>
       </c>
       <c r="F93">
-        <v>556.3200000000001</v>
+        <v>449.81</v>
       </c>
       <c r="G93" t="s">
         <v>77</v>
@@ -13735,16 +13741,16 @@
         <v>101</v>
       </c>
       <c r="C94" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D94" t="s">
         <v>100</v>
       </c>
       <c r="E94">
-        <v>1477.7</v>
+        <v>1357.2</v>
       </c>
       <c r="F94">
-        <v>449.81</v>
+        <v>599.1900000000001</v>
       </c>
       <c r="G94" t="s">
         <v>77</v>
@@ -13755,22 +13761,22 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B95" t="s">
         <v>101</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D95" t="s">
         <v>100</v>
       </c>
       <c r="E95">
-        <v>1357.2</v>
+        <v>2097.9</v>
       </c>
       <c r="F95">
-        <v>599.1900000000001</v>
+        <v>62.309</v>
       </c>
       <c r="G95" t="s">
         <v>77</v>
@@ -13784,19 +13790,19 @@
         <v>34</v>
       </c>
       <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96" t="s">
         <v>101</v>
       </c>
-      <c r="C96" t="s">
-        <v>34</v>
-      </c>
-      <c r="D96" t="s">
-        <v>100</v>
-      </c>
       <c r="E96">
-        <v>2097.9</v>
+        <v>1464.1</v>
       </c>
       <c r="F96">
-        <v>62.309</v>
+        <v>591.55</v>
       </c>
       <c r="G96" t="s">
         <v>77</v>
@@ -13810,19 +13816,19 @@
         <v>34</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
         <v>35</v>
       </c>
       <c r="D97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E97">
-        <v>1464.1</v>
+        <v>2500</v>
       </c>
       <c r="F97">
-        <v>591.55</v>
+        <v>10.444</v>
       </c>
       <c r="G97" t="s">
         <v>77</v>
@@ -13836,19 +13842,19 @@
         <v>34</v>
       </c>
       <c r="B98" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" t="s">
         <v>101</v>
       </c>
-      <c r="C98" t="s">
-        <v>35</v>
-      </c>
-      <c r="D98" t="s">
-        <v>100</v>
-      </c>
       <c r="E98">
-        <v>2500</v>
+        <v>629.88</v>
       </c>
       <c r="F98">
-        <v>10.444</v>
+        <v>346.08</v>
       </c>
       <c r="G98" t="s">
         <v>77</v>
@@ -13862,19 +13868,19 @@
         <v>34</v>
       </c>
       <c r="B99" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C99" t="s">
         <v>36</v>
       </c>
       <c r="D99" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E99">
-        <v>629.88</v>
+        <v>2403.8</v>
       </c>
       <c r="F99">
-        <v>346.08</v>
+        <v>26.192</v>
       </c>
       <c r="G99" t="s">
         <v>77</v>
@@ -13888,19 +13894,19 @@
         <v>34</v>
       </c>
       <c r="B100" t="s">
+        <v>100</v>
+      </c>
+      <c r="C100" t="s">
+        <v>37</v>
+      </c>
+      <c r="D100" t="s">
         <v>101</v>
       </c>
-      <c r="C100" t="s">
-        <v>36</v>
-      </c>
-      <c r="D100" t="s">
-        <v>100</v>
-      </c>
       <c r="E100">
-        <v>2403.8</v>
+        <v>341.13</v>
       </c>
       <c r="F100">
-        <v>26.192</v>
+        <v>1499.8</v>
       </c>
       <c r="G100" t="s">
         <v>77</v>
@@ -13914,19 +13920,19 @@
         <v>34</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C101" t="s">
         <v>37</v>
       </c>
       <c r="D101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E101">
-        <v>341.13</v>
+        <v>1390.1</v>
       </c>
       <c r="F101">
-        <v>1499.8</v>
+        <v>947.9299999999999</v>
       </c>
       <c r="G101" t="s">
         <v>77</v>
@@ -13943,16 +13949,16 @@
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D102" t="s">
         <v>100</v>
       </c>
       <c r="E102">
-        <v>1390.1</v>
+        <v>1247.2</v>
       </c>
       <c r="F102">
-        <v>947.9299999999999</v>
+        <v>286.83</v>
       </c>
       <c r="G102" t="s">
         <v>77</v>
@@ -13966,19 +13972,19 @@
         <v>34</v>
       </c>
       <c r="B103" t="s">
+        <v>100</v>
+      </c>
+      <c r="C103" t="s">
+        <v>43</v>
+      </c>
+      <c r="D103" t="s">
         <v>101</v>
       </c>
-      <c r="C103" t="s">
-        <v>38</v>
-      </c>
-      <c r="D103" t="s">
-        <v>100</v>
-      </c>
       <c r="E103">
-        <v>1247.2</v>
+        <v>2182.7</v>
       </c>
       <c r="F103">
-        <v>286.83</v>
+        <v>402.6</v>
       </c>
       <c r="G103" t="s">
         <v>77</v>
@@ -13992,19 +13998,19 @@
         <v>34</v>
       </c>
       <c r="B104" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C104" t="s">
         <v>43</v>
       </c>
       <c r="D104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E104">
-        <v>2182.7</v>
+        <v>250.03</v>
       </c>
       <c r="F104">
-        <v>402.6</v>
+        <v>25</v>
       </c>
       <c r="G104" t="s">
         <v>77</v>
@@ -14021,16 +14027,16 @@
         <v>101</v>
       </c>
       <c r="C105" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D105" t="s">
         <v>100</v>
       </c>
       <c r="E105">
-        <v>250.03</v>
+        <v>1247.2</v>
       </c>
       <c r="F105">
-        <v>25</v>
+        <v>286.83</v>
       </c>
       <c r="G105" t="s">
         <v>77</v>
@@ -14047,16 +14053,16 @@
         <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D106" t="s">
         <v>100</v>
       </c>
       <c r="E106">
-        <v>1247.2</v>
+        <v>1284.9</v>
       </c>
       <c r="F106">
-        <v>286.83</v>
+        <v>2978.8</v>
       </c>
       <c r="G106" t="s">
         <v>77</v>
@@ -14076,13 +14082,13 @@
         <v>69</v>
       </c>
       <c r="D107" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E107">
-        <v>1284.9</v>
+        <v>3889.3</v>
       </c>
       <c r="F107">
-        <v>2978.8</v>
+        <v>0.43712</v>
       </c>
       <c r="G107" t="s">
         <v>77</v>
@@ -14096,19 +14102,19 @@
         <v>34</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C108" t="s">
         <v>69</v>
       </c>
       <c r="D108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E108">
-        <v>3889.3</v>
+        <v>1284.9</v>
       </c>
       <c r="F108">
-        <v>0.43712</v>
+        <v>2978.8</v>
       </c>
       <c r="G108" t="s">
         <v>77</v>
@@ -14119,22 +14125,22 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B109" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C109" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="D109" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E109">
-        <v>1284.9</v>
+        <v>2480.6</v>
       </c>
       <c r="F109">
-        <v>2978.8</v>
+        <v>8.474</v>
       </c>
       <c r="G109" t="s">
         <v>77</v>
@@ -14151,16 +14157,16 @@
         <v>101</v>
       </c>
       <c r="C110" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D110" t="s">
         <v>100</v>
       </c>
       <c r="E110">
-        <v>2480.6</v>
+        <v>2278.5</v>
       </c>
       <c r="F110">
-        <v>8.474</v>
+        <v>73.69799999999999</v>
       </c>
       <c r="G110" t="s">
         <v>77</v>
@@ -14180,7 +14186,7 @@
         <v>69</v>
       </c>
       <c r="D111" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E111">
         <v>2278.5</v>
@@ -14200,13 +14206,13 @@
         <v>35</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C112" t="s">
         <v>69</v>
       </c>
       <c r="D112" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E112">
         <v>2278.5</v>
@@ -14223,22 +14229,22 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B113" t="s">
         <v>100</v>
       </c>
       <c r="C113" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="D113" t="s">
         <v>101</v>
       </c>
       <c r="E113">
-        <v>2278.5</v>
+        <v>1070.8</v>
       </c>
       <c r="F113">
-        <v>73.69799999999999</v>
+        <v>95.22499999999999</v>
       </c>
       <c r="G113" t="s">
         <v>77</v>
@@ -14252,19 +14258,19 @@
         <v>36</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C114" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D114" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E114">
-        <v>1070.8</v>
+        <v>1639.9</v>
       </c>
       <c r="F114">
-        <v>95.22499999999999</v>
+        <v>37.9</v>
       </c>
       <c r="G114" t="s">
         <v>77</v>
@@ -14278,19 +14284,19 @@
         <v>36</v>
       </c>
       <c r="B115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C115" t="s">
         <v>37</v>
       </c>
       <c r="D115" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E115">
-        <v>1639.9</v>
+        <v>1682.1</v>
       </c>
       <c r="F115">
-        <v>37.9</v>
+        <v>0.582</v>
       </c>
       <c r="G115" t="s">
         <v>77</v>
@@ -14301,7 +14307,7 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B116" t="s">
         <v>100</v>
@@ -14313,10 +14319,10 @@
         <v>101</v>
       </c>
       <c r="E116">
-        <v>1682.1</v>
+        <v>1370.3</v>
       </c>
       <c r="F116">
-        <v>0.582</v>
+        <v>10.062</v>
       </c>
       <c r="G116" t="s">
         <v>77</v>
@@ -14327,22 +14333,22 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B117" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C117" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D117" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E117">
-        <v>1370.3</v>
+        <v>1511.6</v>
       </c>
       <c r="F117">
-        <v>10.062</v>
+        <v>87.651</v>
       </c>
       <c r="G117" t="s">
         <v>77</v>
@@ -14359,16 +14365,16 @@
         <v>101</v>
       </c>
       <c r="C118" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D118" t="s">
         <v>100</v>
       </c>
       <c r="E118">
-        <v>1511.6</v>
+        <v>901.35</v>
       </c>
       <c r="F118">
-        <v>87.651</v>
+        <v>1.1555</v>
       </c>
       <c r="G118" t="s">
         <v>77</v>
@@ -14379,22 +14385,22 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B119" t="s">
+        <v>100</v>
+      </c>
+      <c r="C119" t="s">
+        <v>69</v>
+      </c>
+      <c r="D119" t="s">
         <v>101</v>
       </c>
-      <c r="C119" t="s">
-        <v>40</v>
-      </c>
-      <c r="D119" t="s">
-        <v>100</v>
-      </c>
       <c r="E119">
-        <v>901.35</v>
+        <v>3961.5</v>
       </c>
       <c r="F119">
-        <v>1.1555</v>
+        <v>0.023401</v>
       </c>
       <c r="G119" t="s">
         <v>77</v>
@@ -14405,22 +14411,22 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B120" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C120" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="D120" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E120">
-        <v>3961.5</v>
+        <v>1538.1</v>
       </c>
       <c r="F120">
-        <v>0.023401</v>
+        <v>275.86</v>
       </c>
       <c r="G120" t="s">
         <v>77</v>
@@ -14431,22 +14437,22 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B121" t="s">
+        <v>100</v>
+      </c>
+      <c r="C121" t="s">
+        <v>45</v>
+      </c>
+      <c r="D121" t="s">
         <v>101</v>
       </c>
-      <c r="C121" t="s">
-        <v>43</v>
-      </c>
-      <c r="D121" t="s">
-        <v>100</v>
-      </c>
       <c r="E121">
-        <v>1538.1</v>
+        <v>1293.5</v>
       </c>
       <c r="F121">
-        <v>275.86</v>
+        <v>438.49</v>
       </c>
       <c r="G121" t="s">
         <v>77</v>
@@ -14457,22 +14463,22 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B122" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C122" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D122" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E122">
-        <v>1293.5</v>
+        <v>1492</v>
       </c>
       <c r="F122">
-        <v>438.49</v>
+        <v>76.411</v>
       </c>
       <c r="G122" t="s">
         <v>77</v>
@@ -14489,16 +14495,16 @@
         <v>101</v>
       </c>
       <c r="C123" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D123" t="s">
         <v>100</v>
       </c>
       <c r="E123">
-        <v>1492</v>
+        <v>802.21</v>
       </c>
       <c r="F123">
-        <v>76.411</v>
+        <v>52.555</v>
       </c>
       <c r="G123" t="s">
         <v>77</v>
@@ -14515,16 +14521,16 @@
         <v>101</v>
       </c>
       <c r="C124" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D124" t="s">
         <v>100</v>
       </c>
       <c r="E124">
-        <v>802.21</v>
+        <v>2266</v>
       </c>
       <c r="F124">
-        <v>52.555</v>
+        <v>43.7</v>
       </c>
       <c r="G124" t="s">
         <v>77</v>
@@ -14541,16 +14547,16 @@
         <v>101</v>
       </c>
       <c r="C125" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D125" t="s">
         <v>100</v>
       </c>
       <c r="E125">
-        <v>2266</v>
+        <v>2900</v>
       </c>
       <c r="F125">
-        <v>43.7</v>
+        <v>38.401</v>
       </c>
       <c r="G125" t="s">
         <v>77</v>
@@ -14567,16 +14573,16 @@
         <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D126" t="s">
         <v>100</v>
       </c>
       <c r="E126">
-        <v>2900</v>
+        <v>1398.1</v>
       </c>
       <c r="F126">
-        <v>38.401</v>
+        <v>91.419</v>
       </c>
       <c r="G126" t="s">
         <v>77</v>
@@ -14587,22 +14593,22 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B127" t="s">
         <v>101</v>
       </c>
       <c r="C127" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D127" t="s">
         <v>100</v>
       </c>
       <c r="E127">
-        <v>1398.1</v>
+        <v>1300</v>
       </c>
       <c r="F127">
-        <v>91.419</v>
+        <v>8.9978</v>
       </c>
       <c r="G127" t="s">
         <v>77</v>
@@ -14613,22 +14619,22 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B128" t="s">
         <v>101</v>
       </c>
       <c r="C128" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D128" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E128">
-        <v>1300</v>
+        <v>4745.7</v>
       </c>
       <c r="F128">
-        <v>8.9978</v>
+        <v>10.04</v>
       </c>
       <c r="G128" t="s">
         <v>77</v>
@@ -14645,16 +14651,16 @@
         <v>101</v>
       </c>
       <c r="C129" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D129" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E129">
-        <v>4745.7</v>
+        <v>2424.1</v>
       </c>
       <c r="F129">
-        <v>10.04</v>
+        <v>990.46</v>
       </c>
       <c r="G129" t="s">
         <v>77</v>
@@ -14671,16 +14677,16 @@
         <v>101</v>
       </c>
       <c r="C130" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D130" t="s">
         <v>100</v>
       </c>
       <c r="E130">
-        <v>2424.1</v>
+        <v>2828.1</v>
       </c>
       <c r="F130">
-        <v>990.46</v>
+        <v>47.677</v>
       </c>
       <c r="G130" t="s">
         <v>77</v>
@@ -14691,28 +14697,28 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B131" t="s">
+        <v>100</v>
+      </c>
+      <c r="C131" t="s">
+        <v>29</v>
+      </c>
+      <c r="D131" t="s">
         <v>101</v>
       </c>
-      <c r="C131" t="s">
-        <v>71</v>
-      </c>
-      <c r="D131" t="s">
-        <v>100</v>
-      </c>
       <c r="E131">
-        <v>2828.1</v>
+        <v>1799.8</v>
       </c>
       <c r="F131">
-        <v>47.677</v>
+        <v>125.45</v>
       </c>
       <c r="G131" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="H131" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -15126,7 +15132,7 @@
         <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>87</v>
@@ -15149,7 +15155,7 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D2">
         <v>509.37</v>
@@ -15172,7 +15178,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3">
         <v>780.24</v>
@@ -15195,7 +15201,7 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4">
         <v>358.02</v>
@@ -15218,7 +15224,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D5">
         <v>339.89</v>
@@ -15241,7 +15247,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6">
         <v>134.58</v>
@@ -15264,7 +15270,7 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D7">
         <v>90.008</v>
@@ -15287,7 +15293,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D8">
         <v>1569.8</v>
@@ -15310,7 +15316,7 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>241.18</v>
@@ -15333,7 +15339,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D10">
         <v>488.28</v>
@@ -15375,7 +15381,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>98</v>
@@ -15404,7 +15410,7 @@
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F2">
         <v>600</v>
@@ -15433,7 +15439,7 @@
         <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F3">
         <v>2000.6</v>
@@ -15462,7 +15468,7 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F4">
         <v>1364.4</v>
@@ -15491,7 +15497,7 @@
         <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F5">
         <v>1877.5</v>
@@ -15520,7 +15526,7 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F6">
         <v>3313</v>
@@ -15549,7 +15555,7 @@
         <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F7">
         <v>4943.6</v>
@@ -15578,7 +15584,7 @@
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F8">
         <v>629.88</v>
@@ -15607,7 +15613,7 @@
         <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F9">
         <v>2403.8</v>
@@ -15636,7 +15642,7 @@
         <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F10">
         <v>7020.9</v>
@@ -15665,7 +15671,7 @@
         <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F11">
         <v>2490.6</v>
@@ -15694,7 +15700,7 @@
         <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F12">
         <v>1390.1</v>
@@ -15723,7 +15729,7 @@
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F13">
         <v>341.13</v>
@@ -15752,7 +15758,7 @@
         <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F14">
         <v>2876.5</v>
@@ -15781,7 +15787,7 @@
         <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F15">
         <v>5500.7</v>
@@ -15810,7 +15816,7 @@
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F16">
         <v>3437.4</v>
@@ -15839,7 +15845,7 @@
         <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F17">
         <v>1210.9</v>
@@ -15868,7 +15874,7 @@
         <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F18">
         <v>305.8</v>
@@ -15897,7 +15903,7 @@
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F19">
         <v>1756.2</v>

</xml_diff>

<commit_message>
updated package for new cythonize function
</commit_message>
<xml_diff>
--- a/sgtpy/database/saftgamma_database.xlsx
+++ b/sgtpy/database/saftgamma_database.xlsx
@@ -3702,13 +3702,13 @@
         <v>6</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60">
         <v>0</v>

</xml_diff>